<commit_message>
Quellentabelle - Ich habe die Autoren für die Quellen rausgeschrieben.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D41DC0-A352-44B0-9409-BDC86FC1142E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102A3264-E605-4AD5-AB3E-5182DF64E62F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>Autor</t>
   </si>
@@ -73,9 +73,6 @@
     <t xml:space="preserve"> Some human factors design issues and recommendations for automobile navigation information systems</t>
   </si>
   <si>
-    <t>Failure to detect tactile change: A tactile equivalent to the change blindness phenomenon</t>
-  </si>
-  <si>
     <t>Titel</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
   </si>
   <si>
     <t>Haptische Parameter, Aufmerksamkeit, Affekt, Neuheits Index</t>
-  </si>
-  <si>
-    <t>Hong Z. Tan, Robert Gray, J. Jay Young, and Ryan Traylor</t>
   </si>
   <si>
     <t>Wissenschaftliche Arbeiten\Emulating Human Attention-Getting Practices with Wearable Haptics.pdf</t>
@@ -160,28 +154,46 @@
     </r>
   </si>
   <si>
-    <t>Matthew A. Baumann∗ Karon E. MacLean† Thomas W. Hazelton‡ Ashley McKay§</t>
-  </si>
-  <si>
-    <t>Ying (Jean) Zheng* John B. Morrelli'</t>
-  </si>
-  <si>
-    <t>Lynette A. Jones, Massachusetts Institute of Technology, Cambridge, Massachusetts, and Nadine B. Sarter, University of Michigan, Ann Arbor, Michigan</t>
-  </si>
-  <si>
-    <t>Sevgi Ertan, Clare Lee, Abigail Willets, Hong Tan and Alex Pentland</t>
-  </si>
-  <si>
-    <t>James C. Bliss, Member, IEEE, Michael, H. Katcher, Charles H. Rogers, Member, IEEE, and Raymond P. Shepard</t>
-  </si>
-  <si>
-    <t>Stephen Brewster and Lorna M. Brown</t>
-  </si>
-  <si>
     <t>Lorna M. Brown, Topi Kaaresoja</t>
   </si>
   <si>
     <t>Grega Jakus, Christina Dicke, Jaka Sodnik</t>
+  </si>
+  <si>
+    <t>Ping Li</t>
+  </si>
+  <si>
+    <t>The failure to detect tactile change: A tactile equivalent to the change blindness phenomenon</t>
+  </si>
+  <si>
+    <t>Alberto Gallace, Hong Z. Tan, Charles Spence</t>
+  </si>
+  <si>
+    <t>Francine Gemperle, Nathan Ota, Dan Siewiorek</t>
+  </si>
+  <si>
+    <t>George A. Gescheider, Stanley J. Bolanowski, Jennifer V. Pope, Ronald T. Verrillo</t>
+  </si>
+  <si>
+    <t>Stephen Brewster, Lorna M. Brown</t>
+  </si>
+  <si>
+    <t>Hong Z. Tan, Robert Gray, J. Jay Young, , Ryan Traylor</t>
+  </si>
+  <si>
+    <t>Sevgi Ertan, Clare Lee, Abigail Willets, Hong Tan , Alex Pentl,</t>
+  </si>
+  <si>
+    <t>Matthew A. Baumann, Karon E. MacLean, Thomas W. Hazelton, Ashley McKay</t>
+  </si>
+  <si>
+    <t>Ying (Jean) Zheng, John B. Morrelli'</t>
+  </si>
+  <si>
+    <t>Lynette A. Jones, Nadine B. Sarter, Ann Arbor</t>
+  </si>
+  <si>
+    <t>James C. Bliss, Michael, H. Katcher, Charles H. Rogers, Raymond P. Shepard</t>
   </si>
 </sst>
 </file>
@@ -370,25 +382,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -417,6 +411,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -712,59 +724,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9385"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="12" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="6" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" style="6" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="14" customWidth="1"/>
-    <col min="8" max="8" width="51.140625" style="14" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="11"/>
+    <col min="7" max="7" width="18.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="51.140625" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" s="19" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="18" t="s">
+      <c r="E2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -772,77 +784,77 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>21</v>
       </c>
       <c r="F3" s="2">
         <v>10</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>19</v>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>28</v>
+      <c r="C4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>25</v>
+      <c r="G4" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>29</v>
+      <c r="C5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="F5" s="3">
         <v>10</v>
       </c>
-      <c r="G5" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>30</v>
+      <c r="C6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="F6" s="3">
         <v>5</v>
@@ -852,82 +864,82 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>31</v>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>32</v>
+      <c r="C8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>33</v>
+      <c r="E9" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>34</v>
+      <c r="C10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>35</v>
+      <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -937,11 +949,14 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="13" t="s">
-        <v>36</v>
+      <c r="C12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -951,11 +966,14 @@
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>37</v>
+      <c r="B13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="F13" s="3">
         <v>7</v>
@@ -965,11 +983,14 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>39</v>
+      <c r="B14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F14" s="3">
         <v>8</v>
@@ -979,14 +1000,17 @@
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Quellentabell - Ich habe die Internetquellen eingefügt.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102A3264-E605-4AD5-AB3E-5182DF64E62F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C4E0BC-BBDB-49A9-8385-DEEA09A273B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Autor</t>
   </si>
@@ -195,12 +195,51 @@
   <si>
     <t>James C. Bliss, Michael, H. Katcher, Charles H. Rogers, Raymond P. Shepard</t>
   </si>
+  <si>
+    <t>Emulating human attention-getting practices with wearable haptics - IEEE Conference Publication</t>
+  </si>
+  <si>
+    <t>Haptic actuator design parameters that influence affect and attention - IEEE Conference Publication</t>
+  </si>
+  <si>
+    <t>https://journals.sagepub.com/doi/abs/10.1518/001872008X250638?casa_token=D3nuGwtJMEoAAAAA%3AoG2-aHXGFud8s83Vb4u7fCybKt7tzYNQj_Rl-555szEc5hsTAaKovwILjb65eazQJHi25yAf-t-8Ww&amp;</t>
+  </si>
+  <si>
+    <t>A wearable haptic navigation guidance system - IEEE Conference Publication</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/4081931/</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=976313</t>
+  </si>
+  <si>
+    <t>Feel who's talking</t>
+  </si>
+  <si>
+    <t>Some human factors design issues and recommendations for automobile navigation information systems - ScienceDirect</t>
+  </si>
+  <si>
+    <t>Can attention be directed to opposite locations in different modalities? An ERP study - ScienceDirect</t>
+  </si>
+  <si>
+    <t>The failure to detect tactile change: A tactile analogue of visual change blindness | SpringerLink</t>
+  </si>
+  <si>
+    <t>Design of a wearable tactile display - IEEE Conference Publication</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/abs/10.1080/08990220220131505?casa_token=R_eVGgddTAgAAAAA%3AbLFraXwiVrsx2SAjH7bVeezu5PDWUia3-oUpdnfxiTppORzv4JZff_9dDytNT1sMiUT9B7-JlOo8kA&amp;</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,12 +249,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -249,8 +282,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="45"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,12 +330,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -301,7 +342,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +422,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -379,63 +432,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -724,38 +787,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9385"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="6" customWidth="1"/>
-    <col min="4" max="5" width="20.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="7" customWidth="1"/>
+    <col min="4" max="5" width="20.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="51.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="23" style="9" customWidth="1"/>
+    <col min="8" max="8" width="84.85546875" style="9" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="17" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
-    </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -784,42 +847,45 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="2">
         <v>10</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -827,50 +893,59 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>27</v>
       </c>
       <c r="F5" s="3">
         <v>10</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -881,13 +956,16 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -898,13 +976,16 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -915,13 +996,16 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="D10" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -932,47 +1016,68 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="D11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="D13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="3">
@@ -983,30 +1088,36 @@
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="D14" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="F14" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -47865,8 +47976,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="F3:F1048576">
     <cfRule type="colorScale" priority="3">
@@ -47880,8 +47991,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ToDo">
+  <conditionalFormatting sqref="A2:XFD3 A16:XFD1048576 A4:C15 E4:XFD15 A1:B1 F1 I1:XFD1">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -47900,8 +48011,20 @@
     <hyperlink ref="E13" r:id="rId12" xr:uid="{0360545E-ACB2-45F1-96FE-8F05FB5B497B}"/>
     <hyperlink ref="E14" r:id="rId13" xr:uid="{82018994-9838-4F94-A3A2-02DB60C40426}"/>
     <hyperlink ref="E15" r:id="rId14" xr:uid="{79B55109-29BC-4A55-9450-FD399E9058A4}"/>
+    <hyperlink ref="D4" r:id="rId15" display="https://ieeexplore.ieee.org/abstract/document/5444662" xr:uid="{DCDEC4F8-6620-4C30-BDC2-0E5F0989DB55}"/>
+    <hyperlink ref="D5" r:id="rId16" display="https://ieeexplore.ieee.org/document/6183832" xr:uid="{33C1820C-19EB-46FB-89BF-070D992EABF9}"/>
+    <hyperlink ref="D6" r:id="rId17" xr:uid="{3E85E095-ABC1-47F3-995D-1A94548EA3E3}"/>
+    <hyperlink ref="D7" r:id="rId18" display="https://ieeexplore.ieee.org/abstract/document/729547" xr:uid="{D811C7A9-F1E5-472A-BE08-1B089BF2A566}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{8E9948A9-99A1-4B78-A29B-6C1FD9E0799E}"/>
+    <hyperlink ref="D9" r:id="rId20" xr:uid="{A59EE3AF-4FD4-4E95-B1C1-10075A409EBD}"/>
+    <hyperlink ref="D10" r:id="rId21" display="https://dl.acm.org/citation.cfm?id=1125577" xr:uid="{8D1626D2-9D3E-4F96-9E69-22793F965EC0}"/>
+    <hyperlink ref="D11" r:id="rId22" display="https://www.sciencedirect.com/science/article/pii/0968090X93900095" xr:uid="{302ED850-2202-4AEB-AF12-BE2FB376369E}"/>
+    <hyperlink ref="D12" r:id="rId23" display="https://www.sciencedirect.com/science/article/pii/S1388245799000528" xr:uid="{39CAF4BB-DE23-4C3D-B6C6-D318BFBCCF52}"/>
+    <hyperlink ref="D13" r:id="rId24" display="https://link.springer.com/article/10.3758/BF03193847" xr:uid="{5D6B4E34-1CB8-47C1-805E-C35313CA53A8}"/>
+    <hyperlink ref="D14" r:id="rId25" display="https://ieeexplore.ieee.org/abstract/document/962082" xr:uid="{64014493-5FFB-4126-9A95-7E13A8CB9650}"/>
+    <hyperlink ref="D15" r:id="rId26" xr:uid="{A24B9BE8-F10C-49E3-A109-C0C97C58A83F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
.gitignore - Ich habe die Stilisierungsdateien im Ordner Arbeit von der Versionskontrolle ausgenommen.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C4E0BC-BBDB-49A9-8385-DEEA09A273B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B629201D-95BF-4F84-BD33-A73543B109ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Titel</t>
-  </si>
-  <si>
-    <t>Leistungssteigerung, Beobachtungsaufgabe, Kardinale Richtung</t>
   </si>
   <si>
     <t>https://digital.lib.washington.edu/researchworks/bitstream/handle/1773/34886/he-v3n1.pdf?sequence=1&amp;isAllowed=y</t>
@@ -233,6 +230,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Leistungssteigerung, Beobachtungsaufgabe, Kardinale Richtung,
+Navigation,
+"Sensoren Salzung",
+Phantom Stimulation</t>
   </si>
 </sst>
 </file>
@@ -462,14 +465,8 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -480,25 +477,21 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -789,7 +782,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -800,22 +793,22 @@
     <col min="4" max="5" width="20.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="9" customWidth="1"/>
-    <col min="8" max="8" width="84.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="122.28515625" style="9" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -831,10 +824,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>2</v>
@@ -851,19 +844,19 @@
         <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="F3" s="2">
         <v>10</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -874,19 +867,19 @@
         <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -897,19 +890,19 @@
         <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3">
         <v>10</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -920,13 +913,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3">
         <v>5</v>
@@ -940,16 +933,16 @@
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -960,16 +953,16 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -980,16 +973,16 @@
         <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1000,16 +993,16 @@
         <v>14</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1020,22 +1013,22 @@
         <v>16</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
-      <c r="G11" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>66</v>
+      <c r="G11" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1046,22 +1039,22 @@
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>66</v>
+      <c r="G12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1069,16 +1062,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="D13" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="3">
         <v>7</v>
@@ -1089,16 +1082,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="F14" s="3">
         <v>8</v>
@@ -1109,19 +1102,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
@@ -47992,7 +47985,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD3 A16:XFD1048576 A4:C15 E4:XFD15 A1:B1 F1 I1:XFD1">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ToDo">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Quellentabelle - Ich habe meine Verwendungszwecke erweitert.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B629201D-95BF-4F84-BD33-A73543B109ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946AC918-D356-4445-B5C4-282666E5B311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
   <si>
     <t>Autor</t>
   </si>
@@ -232,10 +232,44 @@
     <t>-</t>
   </si>
   <si>
+    <t>•In dieser Arbeit ist vor allem die gewonnen Reaktionsgeschwindigkeit interessant. Es ist von einer Durchschnittlichen Steigerung von 41% die Rede. Diese Erkenntnis würde ich unter den Bereich "Leistungssteigerung durch redundante Informationen" stellen.
+•In der Arbeit wird diese Idee weiterführend verwendet um ein Navigationssystem anzudenken. Hier werden die Grenzen von der haptischen Informationsaufnahme, des Menschen, ersichtlich. Denn, in der Arbeit, wird beschrieben, dass die Testpersonen Probleme damit hatten gewisse Nuancen zu unterscheiden.
+•Das von Princeton Cutaneous entdeckte Phänomen der "Springenden Stimulation" scheint mir auch erwähnenswert.</t>
+  </si>
+  <si>
     <t>Leistungssteigerung, Beobachtungsaufgabe, Kardinale Richtung,
 Navigation,
-"Sensoren Salzung",
+"Springende Stimulation",
 Phantom Stimulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•In dieser Arbeit wird  versucht die Charakteristik einer "menschlichen" Behrürung festzustellen. Das Erfolgreiche Umsetzen einer solchen Berührung scheint mir bei vielen Aufmerksamkeitssteuerungs-Aufgaben nützlich zu sein.
+•Die verwendeten Aktivierungsprofile, für "ServoSqueeze" und "ServoTap", haben interessante Auswirkungen auf die Effektivität der Informationsvermittlung. Gerade die Unterscheidung zwischen symmetrischen und asymmetrischen Profilen wurde detailliert beschrieben. 
+</t>
+  </si>
+  <si>
+    <t>•Ein Ergebnis dieser Arbeit ist, dass die Materialien, die zur Erzeugung einer Stimulation, eine untergeordnete Rolle spielen. Es ist effektiver über unterschiedliche Aktivierungsprofile Informationen zu übertragen.
+•Die Korrelationen zwischen Aufmerksamkeit, Affekt und Neuheit. Daraus lässt sich beispielsweise schließen, dass es nicht sinnvoll ist mit demselben Aktivierungsprofil sowohl die Aufmerksamkeit eines Menschen zu erhalten und ihm dabei einen positiven Affekt zu vermitteln.
+•Es wird detailliert beschrieben, wie die Änderung einer der Faktoren zu einer Steigerung bzw. Verminderung der Aufmerksamkeit führt. Daraus lassen sich das allgemeine "Rezept" für eine besonders Aufmerksamkeitsfordernde Stimulation erahnen.</t>
+  </si>
+  <si>
+    <t>Vibratese (Haptische Sprache),
+Aufmerksamkeit durch Vibration,
+Frequenzen</t>
+  </si>
+  <si>
+    <t>•In dieser Arbeit wird allgemein beschrieben, welche Möglichkeiten es gibt Anzeigen, auf haptischer Basis, zu bauen und zu verwenden. Der Schwerpunkt liegt hierbei auf Vibrationsanzeigen. Für mich interessant sind hier die Faktoren, die verwendet werden um Aufmerksamkeit zu gewinnen. Diese sind grob: Frequenz, Stärke, Position un Dauer der Vibration</t>
+  </si>
+  <si>
+    <t>Tragbare Navigation,
+Kardinale Richtungen</t>
+  </si>
+  <si>
+    <t>•Diese Arbeit kann ich maximal als erwähnenswerte Anwendung von Navigationssystem auf Haptikbasis verwenden.</t>
+  </si>
+  <si>
+    <t>•Diese Arbeit stellt die Verwendung von haptischer Stimulation zum Ausgleich von Sehschwächen in Aussicht. Das Problem ist das Alter der Arbeit (Erschienen 1970). Viele Probleme die Angesprochen werden sind nicht mehr relevant.
+•Erkenntnise, wie der minimale Buchstabenabstand, den Menschen noch nachvollziehen können, könnte nützlich sein.</t>
   </si>
 </sst>
 </file>
@@ -781,8 +815,10 @@
   <dimension ref="A1:H9385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -792,8 +828,8 @@
     <col min="3" max="3" width="25.7109375" style="7" customWidth="1"/>
     <col min="4" max="5" width="20.42578125" style="7" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" style="9" customWidth="1"/>
-    <col min="8" max="8" width="122.28515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="132" style="9" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -836,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -856,6 +892,9 @@
         <v>10</v>
       </c>
       <c r="G3" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>66</v>
       </c>
     </row>
@@ -881,6 +920,9 @@
       <c r="G4" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="H4" s="9" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -904,6 +946,9 @@
       <c r="G5" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="H5" s="9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -924,6 +969,12 @@
       <c r="F6" s="3">
         <v>5</v>
       </c>
+      <c r="G6" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -941,8 +992,14 @@
       <c r="E7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>22</v>
+      <c r="F7" s="3">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -961,8 +1018,11 @@
       <c r="E8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Quellentabelle - Ich habe die restlichen Verwendungszwecke zu den ersten Wissenschaftlichen Arbeiten, die ich gelesen haben, fertiggestellt.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946AC918-D356-4445-B5C4-282666E5B311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE6AFAE-F0F4-4341-A698-FEC75FDAF6D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Autor</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t xml:space="preserve"> A four-channel analysis of the tactile sensitivity of the fingertip: Frequency selectivity, spatial summation, and temporal summation</t>
-  </si>
-  <si>
-    <t>Todo</t>
   </si>
   <si>
     <t>Tragbare Haptic, Menschliche Kommunikation</t>
@@ -270,6 +267,49 @@
   <si>
     <t>•Diese Arbeit stellt die Verwendung von haptischer Stimulation zum Ausgleich von Sehschwächen in Aussicht. Das Problem ist das Alter der Arbeit (Erschienen 1970). Viele Probleme die Angesprochen werden sind nicht mehr relevant.
 •Erkenntnise, wie der minimale Buchstabenabstand, den Menschen noch nachvollziehen können, könnte nützlich sein.</t>
+  </si>
+  <si>
+    <t>Sehschwäche,
+Haptische Sprache</t>
+  </si>
+  <si>
+    <t>Tastsymbole,
+Informationsübertragung</t>
+  </si>
+  <si>
+    <t>•Hier ist das Alter der Arbeit (Eschienen 1991) wieder ein Problem.
+•Die Kombination von akustischen und haptischen Signalen ist zwar eine interessante Idee, fällt aber nicht ganz in meinen Arbeitsbereich. Eine kurze Erwähnung wäre hier das Maximum</t>
+  </si>
+  <si>
+    <t>Handy,
+Mobile haptic</t>
+  </si>
+  <si>
+    <t>•In dieser Arbeit wird ein Vorschlag zur Erweiterung von, nicht ausschließlich, Handys vorgestellt. Hier wären die Grenzen für solche Möglichkeiten interessant. Wie viele Informationen können verlustfrei vermittelt werden? Wie lang kann eine Nachricht maximal sein? In welchen Situation funktioniert es nicht?</t>
+  </si>
+  <si>
+    <t>•Es geht um die Grenzen der haptischen Aufnahmefähigkeit von Menschen. Aus dieser Arbeit lassen sich gut Risiken für haptische Systeme erkennen.
+•Problematisch ist Oberflächlichkeit der Arbeit. Es lässt sich zwar das Ziel gut erkenne, die Umsetzung und Methodik ist jedoch recht schwer nachzuvollziehen bzw. nicht detailliert erklärt.</t>
+  </si>
+  <si>
+    <t>Unterscheidungsblindheit,
+Ausschließlich haptische Informationsübertragung</t>
+  </si>
+  <si>
+    <t>•In dieser Arbeit sticht für mich besonders die Aussagen über die haptische Assistenz gegenüber der haptischen Information herraus. Gemeint ist, dass es in schwierigen Situation (bsp. Militärische Einsätze) sinnvoll ist haptische Stimulation als redundante Informationsübertragung zu nutzen. Die Alternative, der ausschließlich haptischen Informationsübertragung, ist fehleranfällig.</t>
+  </si>
+  <si>
+    <t>Interaktion mit mobilen Computern,
+Haptik Verwendung unter schweren Bedingungen</t>
+  </si>
+  <si>
+    <t>Finger,
+Kleine haptische Stimulationsfläche</t>
+  </si>
+  <si>
+    <t>•In dieser Arbeit werden, unter anderem, Optimierungsvorschläge für haptische Informationsüberträger vorgestell. So lassen sich schwere Vesten auf Handschuhe reduzieren. Der unterschied der Funktionalität wäre hier noch interessant.
+•Es stellt sich die Frage, ob diese "Optimierungsmöglichkeiten" universell einsetzbar sind. Es ist beispielsweise denkbar, dass kleinere Stimulationsfläche auf dem Rücken als unangenehmer empfunden werden.
+•Die Arbeit legt ihren Schwerpunkt auf Biomechanik.</t>
   </si>
 </sst>
 </file>
@@ -814,11 +854,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9385"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -863,7 +903,7 @@
         <v>20</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>2</v>
@@ -872,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -880,7 +920,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>18</v>
@@ -892,10 +932,10 @@
         <v>10</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -906,22 +946,22 @@
         <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -932,22 +972,22 @@
         <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3">
         <v>10</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -958,22 +998,22 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3">
         <v>5</v>
       </c>
       <c r="G6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -984,22 +1024,22 @@
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="3">
         <v>2</v>
       </c>
       <c r="G7" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1010,19 +1050,22 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="3">
         <v>3</v>
       </c>
+      <c r="G8" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="H8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1033,16 +1076,22 @@
         <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1053,16 +1102,22 @@
         <v>14</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="F10" s="3">
+        <v>7</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1073,22 +1128,22 @@
         <v>16</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1099,22 +1154,22 @@
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1122,19 +1177,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="D13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1142,19 +1203,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="F14" s="3">
         <v>8</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1165,16 +1232,22 @@
         <v>21</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>22</v>
+        <v>36</v>
+      </c>
+      <c r="F15" s="3">
+        <v>6</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Qullen - Ich habe die Sensory Substitution Quelle durchgearbeitet und bewertet.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE6AFAE-F0F4-4341-A698-FEC75FDAF6D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9FCC35-D79E-4466-960D-C1C50CA56B1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
   <si>
     <t>Autor</t>
   </si>
@@ -310,6 +310,28 @@
     <t>•In dieser Arbeit werden, unter anderem, Optimierungsvorschläge für haptische Informationsüberträger vorgestell. So lassen sich schwere Vesten auf Handschuhe reduzieren. Der unterschied der Funktionalität wäre hier noch interessant.
 •Es stellt sich die Frage, ob diese "Optimierungsmöglichkeiten" universell einsetzbar sind. Es ist beispielsweise denkbar, dass kleinere Stimulationsfläche auf dem Rücken als unangenehmer empfunden werden.
 •Die Arbeit legt ihren Schwerpunkt auf Biomechanik.</t>
+  </si>
+  <si>
+    <t>Tactual Displays for Sensory Substitution and Warable Computers</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\Tactual Displays for Sensory Substitution and Warable Computers.pdf</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/citation.cfm?id=1198611</t>
+  </si>
+  <si>
+    <t>Hong Z. Tan, Alex Pentland</t>
+  </si>
+  <si>
+    <t>Tadoma Methode,
+Tragbare Interfaces,
+Unterstützung,
+Sensory Saltation</t>
+  </si>
+  <si>
+    <t>•In dieser Arbeit wird der Effekt der "Sensory Saltation" hergeleitet. Damit ist die Arbeit eine wichtige Grundlage für die Arbeiten die danach kamen.
+•Die Abschnitte über die Tadoma Methode sind ebenfalls hilfreich, da sie einen direkten Einstieg in das Themengebiet der Sinnesersetzung geben.</t>
   </si>
 </sst>
 </file>
@@ -855,10 +877,10 @@
   <dimension ref="A1:H9385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1250,9 +1272,30 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="3">
+        <v>8</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
@@ -48117,7 +48160,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD3 A16:XFD1048576 A4:C15 E4:XFD15 A1:B1 F1 I1:XFD1">
+  <conditionalFormatting sqref="A2:XFD3 A17:XFD1048576 A1:B1 F1 I1:XFD1 A4:C16 E4:XFD16">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",A1)))</formula>
     </cfRule>
@@ -48149,8 +48192,9 @@
     <hyperlink ref="D13" r:id="rId24" display="https://link.springer.com/article/10.3758/BF03193847" xr:uid="{5D6B4E34-1CB8-47C1-805E-C35313CA53A8}"/>
     <hyperlink ref="D14" r:id="rId25" display="https://ieeexplore.ieee.org/abstract/document/962082" xr:uid="{64014493-5FFB-4126-9A95-7E13A8CB9650}"/>
     <hyperlink ref="D15" r:id="rId26" xr:uid="{A24B9BE8-F10C-49E3-A109-C0C97C58A83F}"/>
+    <hyperlink ref="E16" r:id="rId27" xr:uid="{C20C2246-4BAA-41FF-898A-090540109BD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId27"/>
+  <pageSetup orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ich habe Spatially-limited attention to vibrotactile stimulation hinzugefügt. Außerdem habe ich meine Arbeitsorganisation angepasst.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9FCC35-D79E-4466-960D-C1C50CA56B1B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C1EBCB-CF85-40C1-8E7A-7B1704D167C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
   <si>
     <t>Autor</t>
   </si>
@@ -332,6 +332,9 @@
   <si>
     <t>•In dieser Arbeit wird der Effekt der "Sensory Saltation" hergeleitet. Damit ist die Arbeit eine wichtige Grundlage für die Arbeiten die danach kamen.
 •Die Abschnitte über die Tadoma Methode sind ebenfalls hilfreich, da sie einen direkten Einstieg in das Themengebiet der Sinnesersetzung geben.</t>
+  </si>
+  <si>
+    <t>Spatially-limited attention to vibrotactile stimulation</t>
   </si>
 </sst>
 </file>
@@ -877,10 +880,10 @@
   <dimension ref="A1:H9385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1298,82 +1301,85 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Ich habe Wissenschaftliche Arbeit Nr. 15 hinzugefügt und bewertet.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C1EBCB-CF85-40C1-8E7A-7B1704D167C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BE7B7E-2747-4161-8359-9A81CF2AA141}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
   <si>
     <t>Autor</t>
   </si>
@@ -79,9 +79,6 @@
     <t>https://digital.lib.washington.edu/researchworks/bitstream/handle/1773/34886/he-v3n1.pdf?sequence=1&amp;isAllowed=y</t>
   </si>
   <si>
-    <t>Wissenschaftliche Arbeiten\! - A Haptic Back Display for Attentional and Directional Cueing.pdf</t>
-  </si>
-  <si>
     <t>PDF</t>
   </si>
   <si>
@@ -94,43 +91,7 @@
     <t>Haptische Parameter, Aufmerksamkeit, Affekt, Neuheits Index</t>
   </si>
   <si>
-    <t>Wissenschaftliche Arbeiten\Emulating Human Attention-Getting Practices with Wearable Haptics.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\! - Haptic Actuator Design Parameters That Influence Affect and Attention.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\Tactile Displays Guidance for Their Design and Application.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\A wearable haptic navigation guidance system.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\Optical-to-tactile image conversion for the blind..pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\Tactons Structured Tactile Messages for Non-Visual Information Display.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\Feel who is talking Using tactons for mobile phone alerts.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\Some human factors design issues and recommendations for automobile navigation information systems.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\Can attention be directed to opposite locations in different modalities.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\The failure to detect tactile change A tactile analogue of visual change blindness.pdf</t>
-  </si>
-  <si>
     <t>Design of a wearable tactile display</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\Design of a Wearable Tactile Display.pdf</t>
-  </si>
-  <si>
-    <t>Wissenschaftliche Arbeiten\A four channel analysis of the tactile sensitivity of the fingertip frequency selectivity spatial summation and temporal summation.pdf</t>
   </si>
   <si>
     <r>
@@ -315,9 +276,6 @@
     <t>Tactual Displays for Sensory Substitution and Warable Computers</t>
   </si>
   <si>
-    <t>Wissenschaftliche Arbeiten\Tactual Displays for Sensory Substitution and Warable Computers.pdf</t>
-  </si>
-  <si>
     <t>https://dl.acm.org/citation.cfm?id=1198611</t>
   </si>
   <si>
@@ -335,6 +293,64 @@
   </si>
   <si>
     <t>Spatially-limited attention to vibrotactile stimulation</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\1 - A Haptic Back Display for Attentional and Directional Cueing.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\2 - Emulating Human Attention-Getting Practices with Wearable Haptics.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\3 - Haptic Actuator Design Parameters That Influence Affect and Attention.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\4 - Tactile Displays Guidance for Their Design and Application.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\5 - A wearable haptic navigation guidance system.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\6 - Optical-to-tactile image conversion for the blind..pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\7 - Tactons Structured Tactile Messages for Non-Visual Information Display.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\8 - Feel who is talking Using tactons for mobile phone alerts.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\9 - Some human factors design issues and recommendations for automobile navigation information systems.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\10 - Can attention be directed to opposite locations in different modalities.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\11 - The failure to detect tactile change A tactile analogue of visual change blindness.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\12 - Design of a Wearable Tactile Display.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\13 - A four channel analysis of the tactile sensitivity of the fingertip frequency selectivity spatial summation and temporal summation.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\14 - Tactual Displays for Sensory Substitution and Warable Computers.pdf</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\15 - Spatially-limited attention to vibrotactile stimulation.pdf</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.3758/BF03209357</t>
+  </si>
+  <si>
+    <t>Ove Franzen, Joseph Markowitz, John A. Swets</t>
+  </si>
+  <si>
+    <t>Aufmerksamkeitsunterscheidung,
+Kein Vorteil durch Redundanz</t>
+  </si>
+  <si>
+    <t>•Ich könnte hier Bezug darauf nehmen, dass es nicht notwendigerweise ein Vorteil ist möglichst viele Tactoren zu Verwende, wenn man Informationen vermitteln will. Anscheinend hat der Mensch nur begrenzte Möglichkeiten solche Unterschiede festzustellen.</t>
   </si>
 </sst>
 </file>
@@ -880,10 +896,10 @@
   <dimension ref="A1:H9385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -925,10 +941,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>2</v>
@@ -945,22 +961,22 @@
         <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="F3" s="2">
         <v>10</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -971,22 +987,22 @@
         <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -997,22 +1013,22 @@
         <v>9</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="F5" s="3">
         <v>10</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1023,22 +1039,22 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="F6" s="3">
         <v>5</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1049,22 +1065,22 @@
         <v>11</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="F7" s="3">
         <v>2</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1075,22 +1091,22 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="F8" s="3">
         <v>3</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1101,22 +1117,22 @@
         <v>13</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="F9" s="3">
         <v>3</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1127,22 +1143,22 @@
         <v>14</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="F10" s="3">
         <v>7</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1153,22 +1169,22 @@
         <v>16</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1179,48 +1195,48 @@
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="F13" s="3">
         <v>6</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1228,25 +1244,25 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="F14" s="3">
         <v>8</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1254,25 +1270,25 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="F15" s="3">
         <v>6</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1280,106 +1296,124 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F16" s="3">
         <v>8</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="3">
+        <v>6</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -48166,41 +48200,43 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD3 A17:XFD1048576 A1:B1 F1 I1:XFD1 A4:C16 E4:XFD16">
+  <conditionalFormatting sqref="A2:XFD3 A18:XFD1048576 A1:B1 F1 I1:XFD1 A4:C17 E4:XFD17">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ToDo">
       <formula>NOT(ISERROR(SEARCH("ToDo",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{A0EDE707-F431-4C76-9438-91097C59F24C}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{E112E189-5C29-4558-9FFC-8837D9AB6886}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{97E91921-CEFC-4DFF-9EED-BEA635C69900}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{3337A288-83AC-489C-AC11-51108A349D91}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{FB8C0974-1A50-467B-AC58-9F684C3F4821}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{04CB8AAA-7A6C-4C20-91E9-9A2BD4415D17}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{1CFA38BC-59C1-440C-9430-29DA31308340}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{3C68AF26-E6C2-4D01-AA52-7854A4051B5E}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{A3FFAE07-85E8-4A83-964D-98F15AD9D2C5}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{35D54094-50C9-4474-B96F-980226211561}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{459CC656-6D43-4B2B-B00E-6A885CD9D590}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{0360545E-ACB2-45F1-96FE-8F05FB5B497B}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{82018994-9838-4F94-A3A2-02DB60C40426}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{79B55109-29BC-4A55-9450-FD399E9058A4}"/>
-    <hyperlink ref="D4" r:id="rId15" display="https://ieeexplore.ieee.org/abstract/document/5444662" xr:uid="{DCDEC4F8-6620-4C30-BDC2-0E5F0989DB55}"/>
-    <hyperlink ref="D5" r:id="rId16" display="https://ieeexplore.ieee.org/document/6183832" xr:uid="{33C1820C-19EB-46FB-89BF-070D992EABF9}"/>
-    <hyperlink ref="D6" r:id="rId17" xr:uid="{3E85E095-ABC1-47F3-995D-1A94548EA3E3}"/>
-    <hyperlink ref="D7" r:id="rId18" display="https://ieeexplore.ieee.org/abstract/document/729547" xr:uid="{D811C7A9-F1E5-472A-BE08-1B089BF2A566}"/>
-    <hyperlink ref="D8" r:id="rId19" xr:uid="{8E9948A9-99A1-4B78-A29B-6C1FD9E0799E}"/>
-    <hyperlink ref="D9" r:id="rId20" xr:uid="{A59EE3AF-4FD4-4E95-B1C1-10075A409EBD}"/>
-    <hyperlink ref="D10" r:id="rId21" display="https://dl.acm.org/citation.cfm?id=1125577" xr:uid="{8D1626D2-9D3E-4F96-9E69-22793F965EC0}"/>
-    <hyperlink ref="D11" r:id="rId22" display="https://www.sciencedirect.com/science/article/pii/0968090X93900095" xr:uid="{302ED850-2202-4AEB-AF12-BE2FB376369E}"/>
-    <hyperlink ref="D12" r:id="rId23" display="https://www.sciencedirect.com/science/article/pii/S1388245799000528" xr:uid="{39CAF4BB-DE23-4C3D-B6C6-D318BFBCCF52}"/>
-    <hyperlink ref="D13" r:id="rId24" display="https://link.springer.com/article/10.3758/BF03193847" xr:uid="{5D6B4E34-1CB8-47C1-805E-C35313CA53A8}"/>
-    <hyperlink ref="D14" r:id="rId25" display="https://ieeexplore.ieee.org/abstract/document/962082" xr:uid="{64014493-5FFB-4126-9A95-7E13A8CB9650}"/>
-    <hyperlink ref="D15" r:id="rId26" xr:uid="{A24B9BE8-F10C-49E3-A109-C0C97C58A83F}"/>
-    <hyperlink ref="E16" r:id="rId27" xr:uid="{C20C2246-4BAA-41FF-898A-090540109BD6}"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://ieeexplore.ieee.org/abstract/document/5444662" xr:uid="{DCDEC4F8-6620-4C30-BDC2-0E5F0989DB55}"/>
+    <hyperlink ref="D5" r:id="rId3" display="https://ieeexplore.ieee.org/document/6183832" xr:uid="{33C1820C-19EB-46FB-89BF-070D992EABF9}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{3E85E095-ABC1-47F3-995D-1A94548EA3E3}"/>
+    <hyperlink ref="D7" r:id="rId5" display="https://ieeexplore.ieee.org/abstract/document/729547" xr:uid="{D811C7A9-F1E5-472A-BE08-1B089BF2A566}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{8E9948A9-99A1-4B78-A29B-6C1FD9E0799E}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{A59EE3AF-4FD4-4E95-B1C1-10075A409EBD}"/>
+    <hyperlink ref="D10" r:id="rId8" display="https://dl.acm.org/citation.cfm?id=1125577" xr:uid="{8D1626D2-9D3E-4F96-9E69-22793F965EC0}"/>
+    <hyperlink ref="D11" r:id="rId9" display="https://www.sciencedirect.com/science/article/pii/0968090X93900095" xr:uid="{302ED850-2202-4AEB-AF12-BE2FB376369E}"/>
+    <hyperlink ref="D12" r:id="rId10" display="https://www.sciencedirect.com/science/article/pii/S1388245799000528" xr:uid="{39CAF4BB-DE23-4C3D-B6C6-D318BFBCCF52}"/>
+    <hyperlink ref="D13" r:id="rId11" display="https://link.springer.com/article/10.3758/BF03193847" xr:uid="{5D6B4E34-1CB8-47C1-805E-C35313CA53A8}"/>
+    <hyperlink ref="D14" r:id="rId12" display="https://ieeexplore.ieee.org/abstract/document/962082" xr:uid="{64014493-5FFB-4126-9A95-7E13A8CB9650}"/>
+    <hyperlink ref="D15" r:id="rId13" xr:uid="{A24B9BE8-F10C-49E3-A109-C0C97C58A83F}"/>
+    <hyperlink ref="E3" r:id="rId14" xr:uid="{81A3064B-B024-4FD7-A360-FC2E89056CBB}"/>
+    <hyperlink ref="E4" r:id="rId15" xr:uid="{D1A0808E-BA1D-46FE-B051-9206F81E3A7F}"/>
+    <hyperlink ref="E5" r:id="rId16" xr:uid="{DB0BD14D-4451-4577-9017-AF973266F978}"/>
+    <hyperlink ref="E6" r:id="rId17" xr:uid="{D40702A5-F10E-4380-B3D7-4CE701B9551B}"/>
+    <hyperlink ref="E7" r:id="rId18" xr:uid="{08C18F50-A3AF-4F5D-9FB4-E14B55E86B48}"/>
+    <hyperlink ref="E8" r:id="rId19" xr:uid="{9DCDBC86-1C4C-423F-94B8-9E4438B0B825}"/>
+    <hyperlink ref="E9" r:id="rId20" xr:uid="{C06884D5-9E9E-421F-AFB6-896040EC37F8}"/>
+    <hyperlink ref="E10" r:id="rId21" xr:uid="{E13F5E19-471A-4724-8F79-CD5F75476DC4}"/>
+    <hyperlink ref="E11" r:id="rId22" xr:uid="{CC49890F-EBA7-4556-8601-03CF3BB894E5}"/>
+    <hyperlink ref="E12" r:id="rId23" xr:uid="{B5C7DF91-A35E-4DDB-90AF-709AE92DC91F}"/>
+    <hyperlink ref="E13" r:id="rId24" xr:uid="{0A840F91-A244-4891-8D7C-EEA062D51A92}"/>
+    <hyperlink ref="E14" r:id="rId25" xr:uid="{373F47AF-6C1B-4B30-9A3F-C041FEA27824}"/>
+    <hyperlink ref="E15" r:id="rId26" xr:uid="{24BA8F36-B5A7-4AF2-A1BF-D2ECEBE9256D}"/>
+    <hyperlink ref="E17" r:id="rId27" xr:uid="{98D3400C-CB8C-4821-A295-6C81970DF3DC}"/>
+    <hyperlink ref="E16" r:id="rId28" xr:uid="{7E2EC8FF-B832-493A-B5E2-0BD3843E52D2}"/>
+    <hyperlink ref="D17" r:id="rId29" xr:uid="{C64103F5-539B-4B50-9DCD-A9017F895760}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ich habe eine Referenzenbibliothek angelegt. Ich habe die Referenzenformatierung in meine Arbeit integriert. Ich habe alle Überreste aus der llncs Vorlage entfernt. Ich habe Beispieltexte geschrieben. Ich habe den .tex Code kommentiert.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,17 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BE7B7E-2747-4161-8359-9A81CF2AA141}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FCC9E5-56BA-44EC-9B80-5A863C7B0221}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quellenübersicht" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -896,10 +901,10 @@
   <dimension ref="A1:H9385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ich habe alle Referenzen in jabref aufgeführt.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FCC9E5-56BA-44EC-9B80-5A863C7B0221}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF98A77D-19B9-46FE-AE0C-4D540E6150DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -901,10 +901,10 @@
   <dimension ref="A1:H9385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -48240,8 +48240,9 @@
     <hyperlink ref="E17" r:id="rId27" xr:uid="{98D3400C-CB8C-4821-A295-6C81970DF3DC}"/>
     <hyperlink ref="E16" r:id="rId28" xr:uid="{7E2EC8FF-B832-493A-B5E2-0BD3843E52D2}"/>
     <hyperlink ref="D17" r:id="rId29" xr:uid="{C64103F5-539B-4B50-9DCD-A9017F895760}"/>
+    <hyperlink ref="D16" r:id="rId30" xr:uid="{1AB75453-6068-432B-A247-EA623C233B6D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ich habe die weiteren Quellen, die ich herausgesucht habe, in die Bibliothek eingepflegt.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF98A77D-19B9-46FE-AE0C-4D540E6150DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F38EB99-77D3-44EB-A907-A5F1E69FA491}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="110">
   <si>
     <t>Autor</t>
   </si>
@@ -356,6 +356,45 @@
   </si>
   <si>
     <t>•Ich könnte hier Bezug darauf nehmen, dass es nicht notwendigerweise ein Vorteil ist möglichst viele Tactoren zu Verwende, wenn man Informationen vermitteln will. Anscheinend hat der Mensch nur begrenzte Möglichkeiten solche Unterschiede festzustellen.</t>
+  </si>
+  <si>
+    <t>Augmenting spatial awareness with haptic radar</t>
+  </si>
+  <si>
+    <t>Development of a wearable vibrotactile feedback suit for accelerated human motor learning</t>
+  </si>
+  <si>
+    <t>Non-facial and non-verbal affective expression for appearance-constrained robots used in victim management</t>
+  </si>
+  <si>
+    <t>A psychophysical study of sensory saltation with an open response paradigm</t>
+  </si>
+  <si>
+    <t>Dynamic and predictive links between touch and vision</t>
+  </si>
+  <si>
+    <t>Haptic cueing of a visual change-detection task: Implications for multimodal interfaces</t>
+  </si>
+  <si>
+    <t>Utilty of a tactile display for cueing faults</t>
+  </si>
+  <si>
+    <t>Multisensory feedback in support of pilot-automation coordination: the case of uncommanded mode transitions</t>
+  </si>
+  <si>
+    <t>An instrumentation solution for reducing spatial disorientation mishaps</t>
+  </si>
+  <si>
+    <t>Good vibrations: Tactile feedback in support of attention allocation and human-automation coordination in event-driven domains</t>
+  </si>
+  <si>
+    <t>To see or not to see: The need for attention to perceive changes in scenes</t>
+  </si>
+  <si>
+    <t>Contextual cueing: Implicit learning and memory of visual context guides spatial attention</t>
+  </si>
+  <si>
+    <t>Wissenschaftliche Arbeiten\16 - Augmenting spatial awareness with Haptic Radar.pdf</t>
   </si>
 </sst>
 </file>
@@ -901,10 +940,10 @@
   <dimension ref="A1:H9385"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1348,64 +1387,103 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:8" thickBot="1" x14ac:dyDescent="0.3">
@@ -48241,8 +48319,9 @@
     <hyperlink ref="E16" r:id="rId28" xr:uid="{7E2EC8FF-B832-493A-B5E2-0BD3843E52D2}"/>
     <hyperlink ref="D17" r:id="rId29" xr:uid="{C64103F5-539B-4B50-9DCD-A9017F895760}"/>
     <hyperlink ref="D16" r:id="rId30" xr:uid="{1AB75453-6068-432B-A247-EA623C233B6D}"/>
+    <hyperlink ref="E18" r:id="rId31" xr:uid="{5587E970-DBDF-4590-A387-3FC4FF88A979}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ich habe die Quellen angepasst.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F38EB99-77D3-44EB-A907-A5F1E69FA491}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tricuper\iCloudDrive\1 - Student\8. Semester\Wahlbereich\Proseminar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229D1283-E261-49AA-98DE-53F4E2D52099}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quellenübersicht" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -937,13 +942,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:H9385"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Ich habe einen Text für Teilgebiete geschrieben. Ich habe eine Quelle, die Aufmerksamkeit an sich beschreibt hinzugefügt.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8678AC82-1B9E-442A-9646-AD7594BD9DB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ABFEAA-B5E4-440B-93B8-873C949A8249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="166">
   <si>
     <t>Autor</t>
   </si>
@@ -573,6 +572,9 @@
   <si>
     <t>Kann man sich nicht verwendete Literaturreferenzen ausblenden lassen?</t>
   </si>
+  <si>
+    <t>Soll die Selbstständigkeitserklärung in der Arbeit direkt vorkommne, wie in der Einführung ins wissenschaftliche Arbeiten beschrieben?</t>
+  </si>
 </sst>
 </file>
 
@@ -863,6 +865,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -879,15 +890,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1205,17 +1207,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="20" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -48649,18 +48651,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52D4452-F949-4A72-B81D-CD3420F99966}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="19"/>
-    <col min="2" max="2" width="11.42578125" style="26"/>
+    <col min="2" max="2" width="11.42578125" style="20"/>
     <col min="3" max="3" width="41.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" style="21" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="16"/>
   </cols>
   <sheetData>
@@ -48668,13 +48670,13 @@
       <c r="A1" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="20" t="s">
         <v>152</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="21" t="s">
         <v>154</v>
       </c>
     </row>
@@ -48682,7 +48684,7 @@
       <c r="A2" s="17">
         <v>43630</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="22" t="s">
         <v>155</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -48690,7 +48692,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="20" t="s">
         <v>157</v>
       </c>
       <c r="C3" s="18" t="s">
@@ -48698,7 +48700,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="20" t="s">
         <v>155</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -48706,7 +48708,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="20" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -48714,7 +48716,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="20" t="s">
         <v>157</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -48722,7 +48724,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="20" t="s">
         <v>157</v>
       </c>
       <c r="C7" s="18" t="s">
@@ -48733,7 +48735,7 @@
       <c r="A8" s="17">
         <v>43633</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="20" t="s">
         <v>157</v>
       </c>
       <c r="C8" s="18" t="s">
@@ -48741,11 +48743,22 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="20" t="s">
         <v>155</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>43637</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Frage - Neue Frage hinzugefügt.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ABFEAA-B5E4-440B-93B8-873C949A8249}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC27867-0015-40B6-A4C5-7E1F83C5FA7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="167">
   <si>
     <t>Autor</t>
   </si>
@@ -575,6 +575,9 @@
   <si>
     <t>Soll die Selbstständigkeitserklärung in der Arbeit direkt vorkommne, wie in der Einführung ins wissenschaftliche Arbeiten beschrieben?</t>
   </si>
+  <si>
+    <t>Welchen Anteil an neuen Ideen soll meine Arbeit aufweisen?</t>
+  </si>
 </sst>
 </file>
 
@@ -726,7 +729,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -801,12 +804,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -890,6 +921,36 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -48651,10 +48712,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52D4452-F949-4A72-B81D-CD3420F99966}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48723,24 +48784,27 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+    <row r="7" spans="1:4" s="38" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34"/>
+      <c r="B7" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="36" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="D7" s="37"/>
+    </row>
+    <row r="8" spans="1:4" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
         <v>43633</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="30" t="s">
         <v>157</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="31" t="s">
         <v>163</v>
       </c>
+      <c r="D8" s="32"/>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
@@ -48761,8 +48825,20 @@
         <v>165</v>
       </c>
     </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>43641</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Warum und Wie fertig gemacht.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BFD06E-6015-4E55-BB7F-445DD3F30FDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0B3DB6-475F-4959-BC2F-4835B816450A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="214">
   <si>
     <t>Autor</t>
   </si>
@@ -639,12 +639,6 @@
     <t>Haptische Geräte sind noch nicht ausreichend im Alltag vertreten</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Die Theman anhand von Anwendungen zu durchschreiten macht die Arbeit leichter verständlich, da sie die so die Theorie mit der Praxis kombiniert</t>
-  </si>
-  <si>
     <t>Die Sinne von Menschen wiederherstellen zu können, die entwender bei der Geburt oder im Laufe des Lebens beschädigt worden sind, ist ein unumstreitbar positive Leistung</t>
   </si>
   <si>
@@ -674,6 +668,58 @@
   <si>
     <t>Ich will in jedem Abschnitt festhalten, dass es sich um eine Überwachungsaufgabe handelt. Anschließend zeige ich auf, warum dies eine Belastung für die Aufmerksamkeit des ausführenden Menschen ist.(Diese Zwei Punkte bilden sozusagen meinen Obersatz)
 Ich schließe meine Argumentation mit den nützlichen Anwendungen von haptischen Schnittstellen.</t>
+  </si>
+  <si>
+    <t>Überwachungsaufgaben sind eine sinnvolle Einschränkung des Themas</t>
+  </si>
+  <si>
+    <t>Hier werde nich nach den Vorgaben aus dem Seminar in Trichterform eine Einleitung schreiben.</t>
+  </si>
+  <si>
+    <t>Hier werde ich eine Begründung für die Sinnhaftigkeit dieser Unterteilung schreiben</t>
+  </si>
+  <si>
+    <t>Ich werde das allgemeine Gebiet der haptischen Schnittstellen auf mein Thema reduzieren.</t>
+  </si>
+  <si>
+    <t>Ich werde eine saubere Definition mit deren unterschiedlichen Auslegungen erstellen und die Sinnhaftigkeit dieser verteidigen</t>
+  </si>
+  <si>
+    <t>Hier werde ich eine technische Einführung in haptische Geräte erstellen. Diese technischen Details werde ich dann konkretisieren und greifbar machen.</t>
+  </si>
+  <si>
+    <t>Hier werde ich eine Definition von Überwachungsaufgabe erstellen und deren Sinnhaftigkeit begründen. Außerdem werde ich einige Beispiele auserhalb von dem Spektrum dieser Arbeit hinzuziehen, an denen das Problem von Überwachung erkenntlich wird.</t>
+  </si>
+  <si>
+    <t>Die Themen anhand von Anwendungen zu durchschreiten macht die Arbeit leichter verständlich, da sie die so die Theorie mit der Praxis kombiniert</t>
+  </si>
+  <si>
+    <t>Hier werde ich meine Unterteilung rechtfertigen, wahrscheinlich ohne sie nochmal aufzuführen.</t>
+  </si>
+  <si>
+    <t>Ich werde die wichtigesten Sinne (Hören, Sehen, Riechen?) durchgehen und den aktuellen Forschungsstand präsentieren.
+Leicht zu Abstrakt</t>
+  </si>
+  <si>
+    <t>Ich werde mit einer Einführung in die Funktion der menschlichen Kommunikation anfangen. Dann den Normalfall beschreiben. Gefolgt von Menschlichen Hilfsmitteln(Tandemonia).  Anschließend werde ich aufzeigen, wie Taktoren helfen können.</t>
+  </si>
+  <si>
+    <t>Obersatz erklären und Stand der Forschung präsentieren. Anschließend werde ich Kombinationsmöglichkeiten andeuten.</t>
+  </si>
+  <si>
+    <t>Obersatz, Stand der Forschung. Erweiterung</t>
+  </si>
+  <si>
+    <t>Teile die ich in der Anwendung referenziert habe wieder aufgreifen und noch weitere Punkte ansprechen. (Definitionen nochmals abgehen)</t>
+  </si>
+  <si>
+    <t>Automatisch</t>
+  </si>
+  <si>
+    <t>Fachbegriffe</t>
+  </si>
+  <si>
+    <t>Vorlage liegt bereit</t>
   </si>
 </sst>
 </file>
@@ -996,24 +1042,6 @@
     <xf numFmtId="14" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1039,6 +1067,24 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1356,17 +1402,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="22" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" ht="30" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -48919,239 +48965,287 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F26CF2-A24E-4834-B033-B6B1173566C7}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="25" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" style="30" customWidth="1"/>
-    <col min="4" max="4" width="83.140625" style="35" customWidth="1"/>
-    <col min="5" max="5" width="83.140625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="24" customWidth="1"/>
+    <col min="4" max="4" width="83.140625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="83.140625" style="27" customWidth="1"/>
     <col min="6" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="25" t="s">
         <v>151</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="30" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
+      <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="26" t="s">
         <v>182</v>
       </c>
+      <c r="D2" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
+      <c r="A3" s="25">
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>198</v>
+      <c r="D3" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="25" t="s">
         <v>152</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="24" t="s">
         <v>185</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="D4" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="25" t="s">
         <v>162</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="E5" s="27" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>153</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>187</v>
+      <c r="C6" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="25" t="s">
         <v>154</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>188</v>
+      <c r="C7" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="25" t="s">
         <v>155</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="E8" s="33" t="s">
+      <c r="C8" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="E8" s="27" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="C9" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="E9" s="33" t="s">
+      <c r="C9" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="27" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="25" t="s">
         <v>157</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="E10" s="33" t="s">
+      <c r="C10" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="27" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="25" t="s">
         <v>163</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>192</v>
+      <c r="C11" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="25" t="s">
         <v>164</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="E12" s="33" t="s">
+      <c r="C12" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="25" t="s">
         <v>158</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="E13" s="33" t="s">
+      <c r="C13" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="25" t="s">
         <v>159</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>195</v>
+      <c r="C14" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="25" t="s">
         <v>160</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C15" s="30" t="s">
-        <v>196</v>
-      </c>
-      <c r="E15" s="33" t="s">
+      <c r="C15" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" s="27" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="25" t="s">
         <v>161</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" s="33" t="s">
+      <c r="C16" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="E16" s="27" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="27" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="27" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Struktur geändert. Haptische Schnittstellen weitergeschrieben. Quellen bearbeitet.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0B3DB6-475F-4959-BC2F-4835B816450A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C439E03D-AFF0-4639-A601-5726FD7F24FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="213">
   <si>
     <t>Autor</t>
   </si>
@@ -456,34 +456,13 @@
     <t>Gliederungspunkt</t>
   </si>
   <si>
-    <t>3 - Haptic Actuator Design Parameters That Influence Affect and Attention</t>
-  </si>
-  <si>
-    <t>4 - Tactile Displays Guidance for Their Design and Application</t>
-  </si>
-  <si>
     <t>6 - Optical-to-tactile image conversion for the blind.</t>
   </si>
   <si>
     <t>7 - Tactons Structured Tactile Messages for Non-Visual Information Display</t>
   </si>
   <si>
-    <t>14 - Tactual Displays for Sensory Substitution and Warable Computers</t>
-  </si>
-  <si>
-    <t>17 - Development of a Wearable Vibrotactile Feedback Suit</t>
-  </si>
-  <si>
     <t>1 - A Haptic Back Display for Attentional and Directional Cueing</t>
-  </si>
-  <si>
-    <t>5 - A wearable haptic navigation guidance system</t>
-  </si>
-  <si>
-    <t>15 - Spatially-limited attention to vibrotactile stimulation</t>
-  </si>
-  <si>
-    <t>16 - Augmenting spatial awareness with Haptic Radar</t>
   </si>
   <si>
     <t>Datum</t>
@@ -676,9 +655,6 @@
     <t>Hier werde nich nach den Vorgaben aus dem Seminar in Trichterform eine Einleitung schreiben.</t>
   </si>
   <si>
-    <t>Hier werde ich eine Begründung für die Sinnhaftigkeit dieser Unterteilung schreiben</t>
-  </si>
-  <si>
     <t>Ich werde das allgemeine Gebiet der haptischen Schnittstellen auf mein Thema reduzieren.</t>
   </si>
   <si>
@@ -720,6 +696,37 @@
   </si>
   <si>
     <t>Vorlage liegt bereit</t>
+  </si>
+  <si>
+    <t>32 - Nonparametric Measures of Sensory Efficiency for Sustained Monitoring Tasks</t>
+  </si>
+  <si>
+    <t>17 - Development of a Wearable Vibrotactile Feedback Suit
+Als Bsp. Für nicht haptische Redundanz:
+9 - Some human factors design issues and recommendations for automobile navigation information systems</t>
+  </si>
+  <si>
+    <t>Anmerkung: Die Quellenangaben sind so gedacht, das alle nur irgendwie realistisch verwendbaren Quellen aufgelistet sind</t>
+  </si>
+  <si>
+    <t>Hier werde ich eine Begründung für die Sinnhaftigkeit dieser Unterteilung schreiben
+1 - A Haptic Back Display for Attentional and Directional Cueing</t>
+  </si>
+  <si>
+    <t>1 - A Haptic Back Display for Attentional and Directional Cueing
+14 - Tactual Displays for Sensory Substitution and Warable Computers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - A Haptic Back Display for Attentional and Directional Cueing
+2 - Emulating Human Attention-Getting Practices with Wearable Haptics
+3 - Haptic Actuator Design Parameters That Influence Affect and Attention
+28 - Attention and Effort
+</t>
+  </si>
+  <si>
+    <t>1 - A Haptic Back Display for Attentional and Directional Cueing
+3 - Haptic Actuator Design Parameters That Influence Affect and Attention
+4 - Tactile Displays Guidance for Their Design and Application</t>
   </si>
 </sst>
 </file>
@@ -48863,16 +48870,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -48880,50 +48887,50 @@
         <v>43630</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -48931,18 +48938,18 @@
         <v>43633</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -48950,10 +48957,10 @@
         <v>43637</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -48963,10 +48970,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F26CF2-A24E-4834-B033-B6B1173566C7}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48976,277 +48986,271 @@
     <col min="3" max="3" width="45.7109375" style="24" customWidth="1"/>
     <col min="4" max="4" width="83.140625" style="29" customWidth="1"/>
     <col min="5" max="5" width="83.140625" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="15"/>
+    <col min="6" max="6" width="56" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>125</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="25">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="25">
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C11" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="D12" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B14" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="D14" s="29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="B15" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="B16" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="D16" s="29" t="s">
         <v>205</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="E13" s="27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="27" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="27" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Designs angelegt. Grafiken aus Arbeiten herrausgezogen. Kapitel Zuverlässigkeit weitergeschrieben.
</commit_message>
<xml_diff>
--- a/Proseminar - Quellen - Übersicht.xlsx
+++ b/Proseminar - Quellen - Übersicht.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C439E03D-AFF0-4639-A601-5726FD7F24FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA96A502-1F23-4298-A975-699335B03CCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quellenübersicht" sheetId="1" r:id="rId1"/>
-    <sheet name="Fragen" sheetId="3" r:id="rId2"/>
-    <sheet name="Gliederung mit Quellen" sheetId="2" r:id="rId3"/>
+    <sheet name="Gliederung mit Quellen" sheetId="2" r:id="rId2"/>
+    <sheet name="Fragen" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" refMode="R1C1"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="213">
   <si>
     <t>Autor</t>
   </si>
@@ -1389,8 +1389,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:H9385"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
@@ -48852,127 +48852,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52D4452-F949-4A72-B81D-CD3420F99966}">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="18"/>
-    <col min="2" max="2" width="11.42578125" style="19"/>
-    <col min="3" max="3" width="41.140625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="66.42578125" style="20" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
-        <v>43630</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>43633</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
-        <v>43637</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F26CF2-A24E-4834-B033-B6B1173566C7}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -49256,4 +49139,121 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52D4452-F949-4A72-B81D-CD3420F99966}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="18"/>
+    <col min="2" max="2" width="11.42578125" style="19"/>
+    <col min="3" max="3" width="41.140625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="66.42578125" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>43630</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>43633</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
+        <v>43637</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>